<commit_message>
Agrega brazil a prep
</commit_message>
<xml_diff>
--- a/prep/Resultados_Escenario_Baseline.xlsx
+++ b/prep/Resultados_Escenario_Baseline.xlsx
@@ -461,52 +461,52 @@
         <v>18</v>
       </c>
       <c r="B2" t="n">
-        <v>11314873.0447916</v>
+        <v>11554617.8962204</v>
       </c>
       <c r="C2" t="n">
-        <v>10022868.0907353</v>
+        <v>-268947467.421113</v>
       </c>
       <c r="D2" t="n">
-        <v>414827.413106047</v>
+        <v>150420.128107754</v>
       </c>
       <c r="E2" t="n">
-        <v>347380.707926547</v>
+        <v>113487.224209943</v>
       </c>
       <c r="F2" t="n">
-        <v>92953.1888457952</v>
+        <v>278274299.226709</v>
       </c>
       <c r="G2" t="n">
-        <v>440333.896772342</v>
+        <v>278387786.450919</v>
       </c>
       <c r="H2" t="n">
-        <v>16614.8346250421</v>
+        <v>6329.2755529044</v>
       </c>
       <c r="I2" t="n">
-        <v>0.10322197382423</v>
+        <v>0.0407523589586967</v>
       </c>
       <c r="J2" t="n">
-        <v>51005.3356950971</v>
+        <v>65.8656047451074</v>
       </c>
       <c r="K2" t="n">
-        <v>46414.8554825383</v>
+        <v>5993.77003180478</v>
       </c>
       <c r="L2" t="n">
-        <v>63005.3356950971</v>
+        <v>18065.8656047451</v>
       </c>
       <c r="M2" t="n">
-        <v>204028.012257698</v>
+        <v>27093.9020234045</v>
       </c>
       <c r="N2" t="n">
-        <v>198802132.572256</v>
+        <v>280171313.839889</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>891990163.767911</v>
+        <v>1361104165277.77</v>
       </c>
       <c r="Q2" t="n">
-        <v>1090792296.34017</v>
+        <v>1361384336591.61</v>
       </c>
       <c r="R2" t="n">
         <v>303118.169896544</v>
@@ -517,52 +517,52 @@
         <v>18</v>
       </c>
       <c r="B3" t="n">
-        <v>3998416.35304544</v>
+        <v>4037218.5925632</v>
       </c>
       <c r="C3" t="n">
-        <v>3572767.7394857</v>
+        <v>-153492987.85454</v>
       </c>
       <c r="D3" t="n">
-        <v>162853.055233896</v>
+        <v>103281.492049934</v>
       </c>
       <c r="E3" t="n">
-        <v>137143.211332786</v>
+        <v>78385.4398651211</v>
       </c>
       <c r="F3" t="n">
-        <v>32180.8254608798</v>
+        <v>156770400.673036</v>
       </c>
       <c r="G3" t="n">
-        <v>169324.036793666</v>
+        <v>156848786.112901</v>
       </c>
       <c r="H3" t="n">
-        <v>16614.8346250421</v>
+        <v>6329.2755529044</v>
       </c>
       <c r="I3" t="n">
-        <v>0.10322197382423</v>
+        <v>0.0407523589586967</v>
       </c>
       <c r="J3" t="n">
-        <v>51005.3356950971</v>
+        <v>65.8656047451074</v>
       </c>
       <c r="K3" t="n">
-        <v>46414.8554825383</v>
+        <v>5993.77003180478</v>
       </c>
       <c r="L3" t="n">
-        <v>63005.3356950971</v>
+        <v>18065.8656047451</v>
       </c>
       <c r="M3" t="n">
-        <v>204028.012257698</v>
+        <v>27093.9020234045</v>
       </c>
       <c r="N3" t="n">
-        <v>69760309.6589056</v>
+        <v>93485734.7981108</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>308766362.766889</v>
+        <v>766800415826.048</v>
       </c>
       <c r="Q3" t="n">
-        <v>378526672.425794</v>
+        <v>766893901560.847</v>
       </c>
       <c r="R3" t="n">
         <v>303118.169896544</v>

</xml_diff>